<commit_message>
add book1 to BRAND excel1
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panharith/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panharith/Desktop/Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{103EC423-63A9-D94A-B044-1D95FD4A4157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FE5CFA-965C-E54B-ACCA-CECF2C6D8685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{0472B5D4-53A2-CA4B-BBD2-F9D79BC299D9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>A</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE21BF2-F9B7-CE42-AD2E-F2D2B5F9AE4A}">
-  <dimension ref="B6:B8"/>
+  <dimension ref="B6:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,6 +417,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>